<commit_message>
Committed the Walmart Project
</commit_message>
<xml_diff>
--- a/walmarteCom/TestData/TestData_Items.xlsx
+++ b/walmarteCom/TestData/TestData_Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkat/eclipse-workspace/walmarteCom/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8D2908-393A-8E46-9CAE-7C7AECFC94BF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9618E44C-7B25-F342-87CD-65D964AECECB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="460" windowWidth="21080" windowHeight="8260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>